<commit_message>
BF: DragNDrop demo ended on first click
</commit_message>
<xml_diff>
--- a/psychopy/demos/builder/Experiments/dragAndDrop/conditions.xlsx
+++ b/psychopy/demos/builder/Experiments/dragAndDrop/conditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Throwaway\PsychoPy3 Demos\Experiments\dragAndDrop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44797\PycharmProjects\psychopy\psychopy\demos\builder\Experiments\dragAndDrop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{744D70C6-7892-4BF2-A4DF-238702076018}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3A230D-6D54-43AA-8134-D1AAF5396F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34050" yWindow="1185" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="-7680" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -560,7 +560,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -618,10 +618,10 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>300</v>
+        <v>0.3</v>
       </c>
       <c r="C2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="D2" s="3">
         <v>4</v>
@@ -647,10 +647,10 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>300</v>
+        <v>0.3</v>
       </c>
       <c r="C3">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="D3" s="3">
         <v>4</v>
@@ -676,10 +676,10 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>300</v>
+        <v>0.3</v>
       </c>
       <c r="C4">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="D4" s="3">
         <v>4</v>
@@ -705,10 +705,10 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>300</v>
+        <v>0.3</v>
       </c>
       <c r="C5">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="D5" s="3">
         <v>9</v>
@@ -749,10 +749,10 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>300</v>
+        <v>0.3</v>
       </c>
       <c r="C6">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="D6" s="3">
         <v>9</v>
@@ -793,10 +793,10 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>300</v>
+        <v>0.3</v>
       </c>
       <c r="C7">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="D7" s="3">
         <v>9</v>

</xml_diff>